<commit_message>
add models and migrations
</commit_message>
<xml_diff>
--- a/doku/Zeitplan.xlsx
+++ b/doku/Zeitplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\IPA-Test-2\doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663AFCD7-EAA3-482C-8699-AA56797C3D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCD236E-8E07-4827-AFAA-71C8A32FCF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -300,7 +300,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -309,7 +312,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -319,21 +334,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -621,7 +621,7 @@
   <dimension ref="A1:BD46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,166 +632,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9" t="s">
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9" t="s">
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9" t="s">
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9" t="s">
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9" t="s">
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="9"/>
-      <c r="AC1" s="9"/>
-      <c r="AD1" s="9"/>
-      <c r="AE1" s="9" t="s">
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="AF1" s="9"/>
-      <c r="AG1" s="9"/>
-      <c r="AH1" s="9"/>
-      <c r="AI1" s="9" t="s">
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="AJ1" s="9"/>
-      <c r="AK1" s="9"/>
-      <c r="AL1" s="9"/>
-      <c r="AM1" s="9" t="s">
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="16"/>
+      <c r="AL1" s="16"/>
+      <c r="AM1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AN1" s="9"/>
-      <c r="AO1" s="9"/>
-      <c r="AP1" s="9"/>
-      <c r="AQ1" s="17" t="s">
+      <c r="AN1" s="16"/>
+      <c r="AO1" s="16"/>
+      <c r="AP1" s="16"/>
+      <c r="AQ1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="AR1" s="17"/>
-      <c r="AS1" s="17"/>
-      <c r="AT1" s="17"/>
-      <c r="AU1" s="17" t="s">
+      <c r="AR1" s="10"/>
+      <c r="AS1" s="10"/>
+      <c r="AT1" s="10"/>
+      <c r="AU1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AV1" s="17"/>
-      <c r="AW1" s="17"/>
-      <c r="AX1" s="17"/>
+      <c r="AV1" s="10"/>
+      <c r="AW1" s="10"/>
+      <c r="AX1" s="10"/>
     </row>
     <row r="2" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="10">
+      <c r="A2" s="19"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="11">
         <v>44803</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="10">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="11">
         <v>44804</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="10">
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="11">
         <v>44809</v>
       </c>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="10">
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="11">
         <v>44810</v>
       </c>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="10">
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="11">
         <v>44811</v>
       </c>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="10">
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="11">
         <v>44817</v>
       </c>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="10">
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="11">
         <v>44818</v>
       </c>
-      <c r="AB2" s="11"/>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="11"/>
-      <c r="AE2" s="10">
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="12"/>
+      <c r="AD2" s="12"/>
+      <c r="AE2" s="11">
         <v>44823</v>
       </c>
-      <c r="AF2" s="11"/>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="11"/>
-      <c r="AI2" s="10">
+      <c r="AF2" s="12"/>
+      <c r="AG2" s="12"/>
+      <c r="AH2" s="12"/>
+      <c r="AI2" s="11">
         <v>44824</v>
       </c>
-      <c r="AJ2" s="11"/>
-      <c r="AK2" s="11"/>
-      <c r="AL2" s="11"/>
-      <c r="AM2" s="10">
+      <c r="AJ2" s="12"/>
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="12"/>
+      <c r="AM2" s="11">
         <v>44825</v>
       </c>
-      <c r="AN2" s="11"/>
-      <c r="AO2" s="11"/>
-      <c r="AP2" s="11"/>
-      <c r="AQ2" s="10">
+      <c r="AN2" s="12"/>
+      <c r="AO2" s="12"/>
+      <c r="AP2" s="12"/>
+      <c r="AQ2" s="11">
         <v>44830</v>
       </c>
-      <c r="AR2" s="11"/>
-      <c r="AS2" s="11"/>
-      <c r="AT2" s="11"/>
-      <c r="AU2" s="10">
+      <c r="AR2" s="12"/>
+      <c r="AS2" s="12"/>
+      <c r="AT2" s="12"/>
+      <c r="AU2" s="11">
         <v>44831</v>
       </c>
-      <c r="AV2" s="11"/>
-      <c r="AW2" s="11"/>
-      <c r="AX2" s="11"/>
+      <c r="AV2" s="12"/>
+      <c r="AW2" s="12"/>
+      <c r="AX2" s="12"/>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="5"/>
@@ -844,8 +844,8 @@
       <c r="BD3" s="3"/>
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="2"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
@@ -861,8 +861,8 @@
       <c r="BD4" s="2"/>
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="4"/>
@@ -877,8 +877,8 @@
       <c r="AX5" s="8"/>
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="K6" s="8"/>
@@ -891,8 +891,8 @@
       <c r="AX6" s="8"/>
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="17"/>
+      <c r="B7" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="4"/>
@@ -908,8 +908,8 @@
       <c r="AX7" s="8"/>
     </row>
     <row r="8" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="12"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="9"/>
       <c r="D8" s="2"/>
       <c r="I8" s="2"/>
       <c r="K8" s="8"/>
@@ -922,10 +922,10 @@
       <c r="AX8" s="8"/>
     </row>
     <row r="9" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="6"/>
@@ -941,8 +941,8 @@
       <c r="AX9" s="8"/>
     </row>
     <row r="10" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="12"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="9"/>
       <c r="E10" s="2"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
@@ -954,8 +954,8 @@
       <c r="AX10" s="8"/>
     </row>
     <row r="11" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="12" t="s">
+      <c r="A11" s="17"/>
+      <c r="B11" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H11" s="6"/>
@@ -970,8 +970,8 @@
       <c r="AX11" s="8"/>
     </row>
     <row r="12" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="12"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="9"/>
       <c r="E12" s="2"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
@@ -983,8 +983,8 @@
       <c r="AX12" s="8"/>
     </row>
     <row r="13" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="12" t="s">
+      <c r="A13" s="17"/>
+      <c r="B13" s="9" t="s">
         <v>26</v>
       </c>
       <c r="I13" s="6"/>
@@ -1000,8 +1000,8 @@
       <c r="AX13" s="8"/>
     </row>
     <row r="14" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="12"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="9"/>
       <c r="F14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1015,8 +1015,8 @@
       <c r="AX14" s="8"/>
     </row>
     <row r="15" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="12" t="s">
+      <c r="A15" s="17"/>
+      <c r="B15" s="9" t="s">
         <v>25</v>
       </c>
       <c r="J15" s="6"/>
@@ -1031,8 +1031,8 @@
       <c r="AX15" s="8"/>
     </row>
     <row r="16" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="12"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="9"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1046,10 +1046,10 @@
       <c r="AX16" s="8"/>
     </row>
     <row r="17" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="9" t="s">
         <v>27</v>
       </c>
       <c r="K17" s="8"/>
@@ -1064,8 +1064,8 @@
       <c r="AX17" s="8"/>
     </row>
     <row r="18" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="12"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="9"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
       <c r="N18" s="2"/>
@@ -1077,8 +1077,8 @@
       <c r="AX18" s="8"/>
     </row>
     <row r="19" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="12" t="s">
+      <c r="A19" s="17"/>
+      <c r="B19" s="9" t="s">
         <v>28</v>
       </c>
       <c r="K19" s="8"/>
@@ -1094,8 +1094,8 @@
       <c r="AX19" s="8"/>
     </row>
     <row r="20" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="12"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="9"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="N20" s="2"/>
@@ -1107,10 +1107,10 @@
       <c r="AX20" s="8"/>
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="9" t="s">
         <v>31</v>
       </c>
       <c r="K21" s="8"/>
@@ -1124,8 +1124,8 @@
       <c r="AX21" s="8"/>
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
-      <c r="B22" s="12"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="9"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="N22" s="2"/>
@@ -1137,8 +1137,8 @@
       <c r="AX22" s="8"/>
     </row>
     <row r="23" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="12" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="9" t="s">
         <v>32</v>
       </c>
       <c r="K23" s="8"/>
@@ -1153,10 +1153,12 @@
       <c r="AX23" s="8"/>
     </row>
     <row r="24" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="12"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="9"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
       <c r="AE24" s="8"/>
       <c r="AF24" s="8"/>
       <c r="AQ24" s="8"/>
@@ -1165,8 +1167,8 @@
       <c r="AX24" s="8"/>
     </row>
     <row r="25" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="12" t="s">
+      <c r="A25" s="17"/>
+      <c r="B25" s="9" t="s">
         <v>33</v>
       </c>
       <c r="K25" s="8"/>
@@ -1181,10 +1183,11 @@
       <c r="AX25" s="8"/>
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="12"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="9"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
+      <c r="P26" s="2"/>
       <c r="AE26" s="8"/>
       <c r="AF26" s="8"/>
       <c r="AQ26" s="8"/>
@@ -1193,8 +1196,8 @@
       <c r="AX26" s="8"/>
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="12" t="s">
+      <c r="A27" s="17"/>
+      <c r="B27" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K27" s="8"/>
@@ -1208,8 +1211,8 @@
       <c r="AX27" s="8"/>
     </row>
     <row r="28" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="12"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="9"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
       <c r="AE28" s="8"/>
@@ -1220,8 +1223,8 @@
       <c r="AX28" s="8"/>
     </row>
     <row r="29" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="12" t="s">
+      <c r="A29" s="17"/>
+      <c r="B29" s="9" t="s">
         <v>35</v>
       </c>
       <c r="K29" s="8"/>
@@ -1236,8 +1239,8 @@
       <c r="AX29" s="8"/>
     </row>
     <row r="30" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="12"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="9"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
       <c r="AE30" s="8"/>
@@ -1248,8 +1251,8 @@
       <c r="AX30" s="8"/>
     </row>
     <row r="31" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="12" t="s">
+      <c r="A31" s="17"/>
+      <c r="B31" s="9" t="s">
         <v>36</v>
       </c>
       <c r="K31" s="8"/>
@@ -1265,8 +1268,8 @@
       <c r="AX31" s="8"/>
     </row>
     <row r="32" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="12"/>
+      <c r="A32" s="17"/>
+      <c r="B32" s="9"/>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
       <c r="AE32" s="8"/>
@@ -1277,8 +1280,8 @@
       <c r="AX32" s="8"/>
     </row>
     <row r="33" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
-      <c r="B33" s="12" t="s">
+      <c r="A33" s="17"/>
+      <c r="B33" s="9" t="s">
         <v>37</v>
       </c>
       <c r="K33" s="8"/>
@@ -1295,8 +1298,8 @@
       <c r="AX33" s="8"/>
     </row>
     <row r="34" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="12"/>
+      <c r="A34" s="17"/>
+      <c r="B34" s="9"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
       <c r="AE34" s="8"/>
@@ -1307,8 +1310,8 @@
       <c r="AX34" s="8"/>
     </row>
     <row r="35" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="12" t="s">
+      <c r="A35" s="17"/>
+      <c r="B35" s="9" t="s">
         <v>38</v>
       </c>
       <c r="K35" s="8"/>
@@ -1326,8 +1329,8 @@
       <c r="AX35" s="8"/>
     </row>
     <row r="36" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
-      <c r="B36" s="12"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="9"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
       <c r="AE36" s="8"/>
@@ -1338,8 +1341,8 @@
       <c r="AX36" s="8"/>
     </row>
     <row r="37" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
-      <c r="B37" s="12" t="s">
+      <c r="A37" s="17"/>
+      <c r="B37" s="9" t="s">
         <v>39</v>
       </c>
       <c r="K37" s="8"/>
@@ -1354,8 +1357,8 @@
       <c r="AX37" s="8"/>
     </row>
     <row r="38" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
-      <c r="B38" s="12"/>
+      <c r="A38" s="17"/>
+      <c r="B38" s="9"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
       <c r="AE38" s="8"/>
@@ -1366,10 +1369,10 @@
       <c r="AX38" s="8"/>
     </row>
     <row r="39" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="9" t="s">
         <v>40</v>
       </c>
       <c r="K39" s="8"/>
@@ -1384,8 +1387,8 @@
       <c r="AX39" s="8"/>
     </row>
     <row r="40" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
-      <c r="B40" s="12"/>
+      <c r="A40" s="17"/>
+      <c r="B40" s="9"/>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
       <c r="AE40" s="8"/>
@@ -1396,8 +1399,8 @@
       <c r="AX40" s="8"/>
     </row>
     <row r="41" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A41" s="16"/>
-      <c r="B41" s="12" t="s">
+      <c r="A41" s="17"/>
+      <c r="B41" s="9" t="s">
         <v>41</v>
       </c>
       <c r="K41" s="8"/>
@@ -1411,8 +1414,8 @@
       <c r="AX41" s="8"/>
     </row>
     <row r="42" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
-      <c r="B42" s="12"/>
+      <c r="A42" s="17"/>
+      <c r="B42" s="9"/>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
       <c r="AE42" s="8"/>
@@ -1423,8 +1426,8 @@
       <c r="AX42" s="8"/>
     </row>
     <row r="43" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
-      <c r="B43" s="12" t="s">
+      <c r="A43" s="17"/>
+      <c r="B43" s="9" t="s">
         <v>42</v>
       </c>
       <c r="K43" s="8"/>
@@ -1439,8 +1442,8 @@
       <c r="AX43" s="8"/>
     </row>
     <row r="44" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
-      <c r="B44" s="12"/>
+      <c r="A44" s="17"/>
+      <c r="B44" s="9"/>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
       <c r="AE44" s="8"/>
@@ -1451,10 +1454,10 @@
       <c r="AX44" s="8"/>
     </row>
     <row r="45" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="9" t="s">
         <v>43</v>
       </c>
       <c r="K45" s="8"/>
@@ -1471,8 +1474,8 @@
       <c r="AX45" s="8"/>
     </row>
     <row r="46" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
-      <c r="B46" s="12"/>
+      <c r="A46" s="17"/>
+      <c r="B46" s="9"/>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
       <c r="AE46" s="8"/>
@@ -1484,12 +1487,38 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="AE1:AH1"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="W1:Z1"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="AA1:AD1"/>
+    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:A16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A21:A38"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A39:A44"/>
     <mergeCell ref="AQ1:AT1"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="AU1:AX1"/>
@@ -1506,38 +1535,12 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="AM1:AP1"/>
     <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A39:A44"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A9:A16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A21:A38"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="AA1:AD1"/>
-    <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="AE1:AH1"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="W1:Z1"/>
-    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
controllers for category and trophy made
</commit_message>
<xml_diff>
--- a/doku/Zeitplan.xlsx
+++ b/doku/Zeitplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\IPA-Test-2\doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCD236E-8E07-4827-AFAA-71C8A32FCF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8FD779-0E26-4F2B-B8E2-A2AF1F2EE9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -300,16 +300,31 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -319,21 +334,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -621,7 +621,7 @@
   <dimension ref="A1:BD46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,166 +632,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16" t="s">
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16" t="s">
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16" t="s">
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16" t="s">
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16" t="s">
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16" t="s">
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16"/>
-      <c r="AI1" s="16" t="s">
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="16"/>
-      <c r="AL1" s="16"/>
-      <c r="AM1" s="16" t="s">
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="AN1" s="16"/>
-      <c r="AO1" s="16"/>
-      <c r="AP1" s="16"/>
-      <c r="AQ1" s="10" t="s">
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="9"/>
+      <c r="AP1" s="9"/>
+      <c r="AQ1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="10"/>
-      <c r="AT1" s="10"/>
-      <c r="AU1" s="10" t="s">
+      <c r="AR1" s="17"/>
+      <c r="AS1" s="17"/>
+      <c r="AT1" s="17"/>
+      <c r="AU1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="AV1" s="10"/>
-      <c r="AW1" s="10"/>
-      <c r="AX1" s="10"/>
+      <c r="AV1" s="17"/>
+      <c r="AW1" s="17"/>
+      <c r="AX1" s="17"/>
     </row>
     <row r="2" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="11">
+      <c r="A2" s="14"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="10">
         <v>44803</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="11">
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="10">
         <v>44804</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="11">
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="10">
         <v>44809</v>
       </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="11">
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="10">
         <v>44810</v>
       </c>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="11">
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="10">
         <v>44811</v>
       </c>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="11">
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="10">
         <v>44817</v>
       </c>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="11">
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="10">
         <v>44818</v>
       </c>
-      <c r="AB2" s="12"/>
-      <c r="AC2" s="12"/>
-      <c r="AD2" s="12"/>
-      <c r="AE2" s="11">
+      <c r="AB2" s="11"/>
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="11"/>
+      <c r="AE2" s="10">
         <v>44823</v>
       </c>
-      <c r="AF2" s="12"/>
-      <c r="AG2" s="12"/>
-      <c r="AH2" s="12"/>
-      <c r="AI2" s="11">
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="11"/>
+      <c r="AH2" s="11"/>
+      <c r="AI2" s="10">
         <v>44824</v>
       </c>
-      <c r="AJ2" s="12"/>
-      <c r="AK2" s="12"/>
-      <c r="AL2" s="12"/>
-      <c r="AM2" s="11">
+      <c r="AJ2" s="11"/>
+      <c r="AK2" s="11"/>
+      <c r="AL2" s="11"/>
+      <c r="AM2" s="10">
         <v>44825</v>
       </c>
-      <c r="AN2" s="12"/>
-      <c r="AO2" s="12"/>
-      <c r="AP2" s="12"/>
-      <c r="AQ2" s="11">
+      <c r="AN2" s="11"/>
+      <c r="AO2" s="11"/>
+      <c r="AP2" s="11"/>
+      <c r="AQ2" s="10">
         <v>44830</v>
       </c>
-      <c r="AR2" s="12"/>
-      <c r="AS2" s="12"/>
-      <c r="AT2" s="12"/>
-      <c r="AU2" s="11">
+      <c r="AR2" s="11"/>
+      <c r="AS2" s="11"/>
+      <c r="AT2" s="11"/>
+      <c r="AU2" s="10">
         <v>44831</v>
       </c>
-      <c r="AV2" s="12"/>
-      <c r="AW2" s="12"/>
-      <c r="AX2" s="12"/>
+      <c r="AV2" s="11"/>
+      <c r="AW2" s="11"/>
+      <c r="AX2" s="11"/>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="5"/>
@@ -844,8 +844,8 @@
       <c r="BD3" s="3"/>
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="9"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="2"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
@@ -861,8 +861,8 @@
       <c r="BD4" s="2"/>
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="4"/>
@@ -877,8 +877,8 @@
       <c r="AX5" s="8"/>
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="9"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="K6" s="8"/>
@@ -891,8 +891,8 @@
       <c r="AX6" s="8"/>
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="12" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="4"/>
@@ -908,8 +908,8 @@
       <c r="AX7" s="8"/>
     </row>
     <row r="8" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="12"/>
       <c r="D8" s="2"/>
       <c r="I8" s="2"/>
       <c r="K8" s="8"/>
@@ -922,10 +922,10 @@
       <c r="AX8" s="8"/>
     </row>
     <row r="9" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="12" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="6"/>
@@ -941,8 +941,8 @@
       <c r="AX9" s="8"/>
     </row>
     <row r="10" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="9"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="12"/>
       <c r="E10" s="2"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
@@ -954,8 +954,8 @@
       <c r="AX10" s="8"/>
     </row>
     <row r="11" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="12" t="s">
         <v>24</v>
       </c>
       <c r="H11" s="6"/>
@@ -970,8 +970,8 @@
       <c r="AX11" s="8"/>
     </row>
     <row r="12" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="9"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="12"/>
       <c r="E12" s="2"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
@@ -983,8 +983,8 @@
       <c r="AX12" s="8"/>
     </row>
     <row r="13" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="16"/>
+      <c r="B13" s="12" t="s">
         <v>26</v>
       </c>
       <c r="I13" s="6"/>
@@ -1000,8 +1000,8 @@
       <c r="AX13" s="8"/>
     </row>
     <row r="14" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="9"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="12"/>
       <c r="F14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1015,8 +1015,8 @@
       <c r="AX14" s="8"/>
     </row>
     <row r="15" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="9" t="s">
+      <c r="A15" s="16"/>
+      <c r="B15" s="12" t="s">
         <v>25</v>
       </c>
       <c r="J15" s="6"/>
@@ -1031,8 +1031,8 @@
       <c r="AX15" s="8"/>
     </row>
     <row r="16" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="9"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="12"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1046,10 +1046,10 @@
       <c r="AX16" s="8"/>
     </row>
     <row r="17" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="12" t="s">
         <v>27</v>
       </c>
       <c r="K17" s="8"/>
@@ -1064,8 +1064,8 @@
       <c r="AX17" s="8"/>
     </row>
     <row r="18" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="9"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="12"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
       <c r="N18" s="2"/>
@@ -1077,8 +1077,8 @@
       <c r="AX18" s="8"/>
     </row>
     <row r="19" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="9" t="s">
+      <c r="A19" s="16"/>
+      <c r="B19" s="12" t="s">
         <v>28</v>
       </c>
       <c r="K19" s="8"/>
@@ -1094,8 +1094,8 @@
       <c r="AX19" s="8"/>
     </row>
     <row r="20" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="9"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="12"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="N20" s="2"/>
@@ -1107,10 +1107,10 @@
       <c r="AX20" s="8"/>
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="12" t="s">
         <v>31</v>
       </c>
       <c r="K21" s="8"/>
@@ -1124,8 +1124,8 @@
       <c r="AX21" s="8"/>
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="9"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="12"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="N22" s="2"/>
@@ -1137,8 +1137,8 @@
       <c r="AX22" s="8"/>
     </row>
     <row r="23" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="9" t="s">
+      <c r="A23" s="16"/>
+      <c r="B23" s="12" t="s">
         <v>32</v>
       </c>
       <c r="K23" s="8"/>
@@ -1153,8 +1153,8 @@
       <c r="AX23" s="8"/>
     </row>
     <row r="24" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="9"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="12"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
       <c r="O24" s="2"/>
@@ -1167,8 +1167,8 @@
       <c r="AX24" s="8"/>
     </row>
     <row r="25" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="9" t="s">
+      <c r="A25" s="16"/>
+      <c r="B25" s="12" t="s">
         <v>33</v>
       </c>
       <c r="K25" s="8"/>
@@ -1183,11 +1183,12 @@
       <c r="AX25" s="8"/>
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="9"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="12"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
       <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
       <c r="AE26" s="8"/>
       <c r="AF26" s="8"/>
       <c r="AQ26" s="8"/>
@@ -1196,8 +1197,8 @@
       <c r="AX26" s="8"/>
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="9" t="s">
+      <c r="A27" s="16"/>
+      <c r="B27" s="12" t="s">
         <v>34</v>
       </c>
       <c r="K27" s="8"/>
@@ -1211,10 +1212,12 @@
       <c r="AX27" s="8"/>
     </row>
     <row r="28" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="9"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="12"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
       <c r="AE28" s="8"/>
       <c r="AF28" s="8"/>
       <c r="AQ28" s="8"/>
@@ -1223,8 +1226,8 @@
       <c r="AX28" s="8"/>
     </row>
     <row r="29" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="9" t="s">
+      <c r="A29" s="16"/>
+      <c r="B29" s="12" t="s">
         <v>35</v>
       </c>
       <c r="K29" s="8"/>
@@ -1239,8 +1242,8 @@
       <c r="AX29" s="8"/>
     </row>
     <row r="30" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="9"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="12"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
       <c r="AE30" s="8"/>
@@ -1251,8 +1254,8 @@
       <c r="AX30" s="8"/>
     </row>
     <row r="31" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="9" t="s">
+      <c r="A31" s="16"/>
+      <c r="B31" s="12" t="s">
         <v>36</v>
       </c>
       <c r="K31" s="8"/>
@@ -1268,10 +1271,11 @@
       <c r="AX31" s="8"/>
     </row>
     <row r="32" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="9"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="12"/>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
+      <c r="R32" s="2"/>
       <c r="AE32" s="8"/>
       <c r="AF32" s="8"/>
       <c r="AQ32" s="8"/>
@@ -1280,8 +1284,8 @@
       <c r="AX32" s="8"/>
     </row>
     <row r="33" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="B33" s="9" t="s">
+      <c r="A33" s="16"/>
+      <c r="B33" s="12" t="s">
         <v>37</v>
       </c>
       <c r="K33" s="8"/>
@@ -1298,8 +1302,8 @@
       <c r="AX33" s="8"/>
     </row>
     <row r="34" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
-      <c r="B34" s="9"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="12"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
       <c r="AE34" s="8"/>
@@ -1310,8 +1314,8 @@
       <c r="AX34" s="8"/>
     </row>
     <row r="35" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
-      <c r="B35" s="9" t="s">
+      <c r="A35" s="16"/>
+      <c r="B35" s="12" t="s">
         <v>38</v>
       </c>
       <c r="K35" s="8"/>
@@ -1329,8 +1333,8 @@
       <c r="AX35" s="8"/>
     </row>
     <row r="36" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="B36" s="9"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="12"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
       <c r="AE36" s="8"/>
@@ -1341,8 +1345,8 @@
       <c r="AX36" s="8"/>
     </row>
     <row r="37" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
-      <c r="B37" s="9" t="s">
+      <c r="A37" s="16"/>
+      <c r="B37" s="12" t="s">
         <v>39</v>
       </c>
       <c r="K37" s="8"/>
@@ -1357,8 +1361,8 @@
       <c r="AX37" s="8"/>
     </row>
     <row r="38" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="12"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
       <c r="AE38" s="8"/>
@@ -1369,10 +1373,10 @@
       <c r="AX38" s="8"/>
     </row>
     <row r="39" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="12" t="s">
         <v>40</v>
       </c>
       <c r="K39" s="8"/>
@@ -1387,8 +1391,8 @@
       <c r="AX39" s="8"/>
     </row>
     <row r="40" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="12"/>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
       <c r="AE40" s="8"/>
@@ -1399,8 +1403,8 @@
       <c r="AX40" s="8"/>
     </row>
     <row r="41" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
-      <c r="B41" s="9" t="s">
+      <c r="A41" s="16"/>
+      <c r="B41" s="12" t="s">
         <v>41</v>
       </c>
       <c r="K41" s="8"/>
@@ -1414,8 +1418,8 @@
       <c r="AX41" s="8"/>
     </row>
     <row r="42" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="12"/>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
       <c r="AE42" s="8"/>
@@ -1426,8 +1430,8 @@
       <c r="AX42" s="8"/>
     </row>
     <row r="43" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
-      <c r="B43" s="9" t="s">
+      <c r="A43" s="16"/>
+      <c r="B43" s="12" t="s">
         <v>42</v>
       </c>
       <c r="K43" s="8"/>
@@ -1442,8 +1446,8 @@
       <c r="AX43" s="8"/>
     </row>
     <row r="44" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
-      <c r="B44" s="9"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="12"/>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
       <c r="AE44" s="8"/>
@@ -1454,10 +1458,10 @@
       <c r="AX44" s="8"/>
     </row>
     <row r="45" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="12" t="s">
         <v>43</v>
       </c>
       <c r="K45" s="8"/>
@@ -1474,8 +1478,8 @@
       <c r="AX45" s="8"/>
     </row>
     <row r="46" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
-      <c r="B46" s="9"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="12"/>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
       <c r="AE46" s="8"/>
@@ -1487,38 +1491,12 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="AE1:AH1"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="W1:Z1"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="AA1:AD1"/>
-    <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A9:A16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A21:A38"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
     <mergeCell ref="AQ1:AT1"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="AU1:AX1"/>
@@ -1535,12 +1513,38 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="AM1:AP1"/>
     <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:A16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A21:A38"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="AA1:AD1"/>
+    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="AE1:AH1"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="W1:Z1"/>
+    <mergeCell ref="W2:Z2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
validations and error messages added
</commit_message>
<xml_diff>
--- a/doku/Zeitplan.xlsx
+++ b/doku/Zeitplan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\IPA-Test-2\doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08B84AB-D751-4B3E-93F1-6F278D12507D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239BB560-5214-44AD-BBC1-827F465BD176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -300,16 +300,31 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -319,21 +334,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -621,7 +621,7 @@
   <dimension ref="A1:BD46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U32" sqref="U32"/>
+      <selection activeCell="Y34" sqref="Y34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,166 +632,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16" t="s">
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16" t="s">
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16" t="s">
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16" t="s">
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16" t="s">
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16" t="s">
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16"/>
-      <c r="AI1" s="16" t="s">
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="16"/>
-      <c r="AL1" s="16"/>
-      <c r="AM1" s="16" t="s">
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="AN1" s="16"/>
-      <c r="AO1" s="16"/>
-      <c r="AP1" s="16"/>
-      <c r="AQ1" s="10" t="s">
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="9"/>
+      <c r="AP1" s="9"/>
+      <c r="AQ1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="10"/>
-      <c r="AT1" s="10"/>
-      <c r="AU1" s="10" t="s">
+      <c r="AR1" s="17"/>
+      <c r="AS1" s="17"/>
+      <c r="AT1" s="17"/>
+      <c r="AU1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="AV1" s="10"/>
-      <c r="AW1" s="10"/>
-      <c r="AX1" s="10"/>
+      <c r="AV1" s="17"/>
+      <c r="AW1" s="17"/>
+      <c r="AX1" s="17"/>
     </row>
     <row r="2" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="11">
+      <c r="A2" s="14"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="10">
         <v>44803</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="11">
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="10">
         <v>44804</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="11">
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="10">
         <v>44809</v>
       </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="11">
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="10">
         <v>44810</v>
       </c>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="11">
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="10">
         <v>44811</v>
       </c>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="11">
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="10">
         <v>44817</v>
       </c>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="11">
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="10">
         <v>44818</v>
       </c>
-      <c r="AB2" s="12"/>
-      <c r="AC2" s="12"/>
-      <c r="AD2" s="12"/>
-      <c r="AE2" s="11">
+      <c r="AB2" s="11"/>
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="11"/>
+      <c r="AE2" s="10">
         <v>44823</v>
       </c>
-      <c r="AF2" s="12"/>
-      <c r="AG2" s="12"/>
-      <c r="AH2" s="12"/>
-      <c r="AI2" s="11">
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="11"/>
+      <c r="AH2" s="11"/>
+      <c r="AI2" s="10">
         <v>44824</v>
       </c>
-      <c r="AJ2" s="12"/>
-      <c r="AK2" s="12"/>
-      <c r="AL2" s="12"/>
-      <c r="AM2" s="11">
+      <c r="AJ2" s="11"/>
+      <c r="AK2" s="11"/>
+      <c r="AL2" s="11"/>
+      <c r="AM2" s="10">
         <v>44825</v>
       </c>
-      <c r="AN2" s="12"/>
-      <c r="AO2" s="12"/>
-      <c r="AP2" s="12"/>
-      <c r="AQ2" s="11">
+      <c r="AN2" s="11"/>
+      <c r="AO2" s="11"/>
+      <c r="AP2" s="11"/>
+      <c r="AQ2" s="10">
         <v>44830</v>
       </c>
-      <c r="AR2" s="12"/>
-      <c r="AS2" s="12"/>
-      <c r="AT2" s="12"/>
-      <c r="AU2" s="11">
+      <c r="AR2" s="11"/>
+      <c r="AS2" s="11"/>
+      <c r="AT2" s="11"/>
+      <c r="AU2" s="10">
         <v>44831</v>
       </c>
-      <c r="AV2" s="12"/>
-      <c r="AW2" s="12"/>
-      <c r="AX2" s="12"/>
+      <c r="AV2" s="11"/>
+      <c r="AW2" s="11"/>
+      <c r="AX2" s="11"/>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="5"/>
@@ -844,8 +844,8 @@
       <c r="BD3" s="3"/>
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="9"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="2"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
@@ -861,8 +861,8 @@
       <c r="BD4" s="2"/>
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="4"/>
@@ -877,8 +877,8 @@
       <c r="AX5" s="8"/>
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="9"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="K6" s="8"/>
@@ -891,8 +891,8 @@
       <c r="AX6" s="8"/>
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="12" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="4"/>
@@ -908,8 +908,8 @@
       <c r="AX7" s="8"/>
     </row>
     <row r="8" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="12"/>
       <c r="D8" s="2"/>
       <c r="I8" s="2"/>
       <c r="K8" s="8"/>
@@ -922,10 +922,10 @@
       <c r="AX8" s="8"/>
     </row>
     <row r="9" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="12" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="6"/>
@@ -941,8 +941,8 @@
       <c r="AX9" s="8"/>
     </row>
     <row r="10" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="9"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="12"/>
       <c r="E10" s="2"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
@@ -954,8 +954,8 @@
       <c r="AX10" s="8"/>
     </row>
     <row r="11" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="12" t="s">
         <v>24</v>
       </c>
       <c r="H11" s="6"/>
@@ -970,8 +970,8 @@
       <c r="AX11" s="8"/>
     </row>
     <row r="12" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="9"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="12"/>
       <c r="E12" s="2"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
@@ -983,8 +983,8 @@
       <c r="AX12" s="8"/>
     </row>
     <row r="13" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="16"/>
+      <c r="B13" s="12" t="s">
         <v>26</v>
       </c>
       <c r="I13" s="6"/>
@@ -1000,8 +1000,8 @@
       <c r="AX13" s="8"/>
     </row>
     <row r="14" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="9"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="12"/>
       <c r="F14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1015,8 +1015,8 @@
       <c r="AX14" s="8"/>
     </row>
     <row r="15" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="9" t="s">
+      <c r="A15" s="16"/>
+      <c r="B15" s="12" t="s">
         <v>25</v>
       </c>
       <c r="J15" s="6"/>
@@ -1031,8 +1031,8 @@
       <c r="AX15" s="8"/>
     </row>
     <row r="16" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="9"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="12"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1046,10 +1046,10 @@
       <c r="AX16" s="8"/>
     </row>
     <row r="17" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="12" t="s">
         <v>27</v>
       </c>
       <c r="K17" s="8"/>
@@ -1064,8 +1064,8 @@
       <c r="AX17" s="8"/>
     </row>
     <row r="18" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="9"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="12"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
       <c r="N18" s="2"/>
@@ -1077,8 +1077,8 @@
       <c r="AX18" s="8"/>
     </row>
     <row r="19" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="9" t="s">
+      <c r="A19" s="16"/>
+      <c r="B19" s="12" t="s">
         <v>28</v>
       </c>
       <c r="K19" s="8"/>
@@ -1094,8 +1094,8 @@
       <c r="AX19" s="8"/>
     </row>
     <row r="20" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="9"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="12"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="N20" s="2"/>
@@ -1107,10 +1107,10 @@
       <c r="AX20" s="8"/>
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="12" t="s">
         <v>31</v>
       </c>
       <c r="K21" s="8"/>
@@ -1124,8 +1124,8 @@
       <c r="AX21" s="8"/>
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="9"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="12"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="N22" s="2"/>
@@ -1137,8 +1137,8 @@
       <c r="AX22" s="8"/>
     </row>
     <row r="23" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="9" t="s">
+      <c r="A23" s="16"/>
+      <c r="B23" s="12" t="s">
         <v>32</v>
       </c>
       <c r="K23" s="8"/>
@@ -1153,8 +1153,8 @@
       <c r="AX23" s="8"/>
     </row>
     <row r="24" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="9"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="12"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
       <c r="O24" s="2"/>
@@ -1167,8 +1167,8 @@
       <c r="AX24" s="8"/>
     </row>
     <row r="25" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="9" t="s">
+      <c r="A25" s="16"/>
+      <c r="B25" s="12" t="s">
         <v>33</v>
       </c>
       <c r="K25" s="8"/>
@@ -1183,8 +1183,8 @@
       <c r="AX25" s="8"/>
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="9"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="12"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
       <c r="P26" s="2"/>
@@ -1197,8 +1197,8 @@
       <c r="AX26" s="8"/>
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="9" t="s">
+      <c r="A27" s="16"/>
+      <c r="B27" s="12" t="s">
         <v>34</v>
       </c>
       <c r="K27" s="8"/>
@@ -1212,8 +1212,8 @@
       <c r="AX27" s="8"/>
     </row>
     <row r="28" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="9"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="12"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
       <c r="Q28" s="2"/>
@@ -1226,8 +1226,8 @@
       <c r="AX28" s="8"/>
     </row>
     <row r="29" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="9" t="s">
+      <c r="A29" s="16"/>
+      <c r="B29" s="12" t="s">
         <v>35</v>
       </c>
       <c r="K29" s="8"/>
@@ -1242,8 +1242,8 @@
       <c r="AX29" s="8"/>
     </row>
     <row r="30" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="9"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="12"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
       <c r="S30" s="2"/>
@@ -1256,8 +1256,8 @@
       <c r="AX30" s="8"/>
     </row>
     <row r="31" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="9" t="s">
+      <c r="A31" s="16"/>
+      <c r="B31" s="12" t="s">
         <v>36</v>
       </c>
       <c r="K31" s="8"/>
@@ -1273,8 +1273,8 @@
       <c r="AX31" s="8"/>
     </row>
     <row r="32" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="9"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="12"/>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
       <c r="R32" s="2"/>
@@ -1288,8 +1288,8 @@
       <c r="AX32" s="8"/>
     </row>
     <row r="33" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="B33" s="9" t="s">
+      <c r="A33" s="16"/>
+      <c r="B33" s="12" t="s">
         <v>37</v>
       </c>
       <c r="K33" s="8"/>
@@ -1306,10 +1306,12 @@
       <c r="AX33" s="8"/>
     </row>
     <row r="34" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
-      <c r="B34" s="9"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="12"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
       <c r="AE34" s="8"/>
       <c r="AF34" s="8"/>
       <c r="AQ34" s="8"/>
@@ -1318,8 +1320,8 @@
       <c r="AX34" s="8"/>
     </row>
     <row r="35" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
-      <c r="B35" s="9" t="s">
+      <c r="A35" s="16"/>
+      <c r="B35" s="12" t="s">
         <v>38</v>
       </c>
       <c r="K35" s="8"/>
@@ -1337,8 +1339,8 @@
       <c r="AX35" s="8"/>
     </row>
     <row r="36" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="B36" s="9"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="12"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
       <c r="AE36" s="8"/>
@@ -1349,8 +1351,8 @@
       <c r="AX36" s="8"/>
     </row>
     <row r="37" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
-      <c r="B37" s="9" t="s">
+      <c r="A37" s="16"/>
+      <c r="B37" s="12" t="s">
         <v>39</v>
       </c>
       <c r="K37" s="8"/>
@@ -1365,8 +1367,8 @@
       <c r="AX37" s="8"/>
     </row>
     <row r="38" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="12"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
       <c r="AE38" s="8"/>
@@ -1377,10 +1379,10 @@
       <c r="AX38" s="8"/>
     </row>
     <row r="39" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="12" t="s">
         <v>40</v>
       </c>
       <c r="K39" s="8"/>
@@ -1395,8 +1397,8 @@
       <c r="AX39" s="8"/>
     </row>
     <row r="40" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="12"/>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
       <c r="AE40" s="8"/>
@@ -1407,8 +1409,8 @@
       <c r="AX40" s="8"/>
     </row>
     <row r="41" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
-      <c r="B41" s="9" t="s">
+      <c r="A41" s="16"/>
+      <c r="B41" s="12" t="s">
         <v>41</v>
       </c>
       <c r="K41" s="8"/>
@@ -1422,8 +1424,8 @@
       <c r="AX41" s="8"/>
     </row>
     <row r="42" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="12"/>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
       <c r="AE42" s="8"/>
@@ -1434,8 +1436,8 @@
       <c r="AX42" s="8"/>
     </row>
     <row r="43" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
-      <c r="B43" s="9" t="s">
+      <c r="A43" s="16"/>
+      <c r="B43" s="12" t="s">
         <v>42</v>
       </c>
       <c r="K43" s="8"/>
@@ -1450,8 +1452,8 @@
       <c r="AX43" s="8"/>
     </row>
     <row r="44" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
-      <c r="B44" s="9"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="12"/>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
       <c r="AE44" s="8"/>
@@ -1462,10 +1464,10 @@
       <c r="AX44" s="8"/>
     </row>
     <row r="45" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="12" t="s">
         <v>43</v>
       </c>
       <c r="K45" s="8"/>
@@ -1482,8 +1484,8 @@
       <c r="AX45" s="8"/>
     </row>
     <row r="46" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
-      <c r="B46" s="9"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="12"/>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
       <c r="AE46" s="8"/>
@@ -1495,38 +1497,12 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="AE1:AH1"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="W1:Z1"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="AA1:AD1"/>
-    <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A9:A16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A21:A38"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
     <mergeCell ref="AQ1:AT1"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="AU1:AX1"/>
@@ -1543,12 +1519,38 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="AM1:AP1"/>
     <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:A16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A21:A38"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="AA1:AD1"/>
+    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="AE1:AH1"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="W1:Z1"/>
+    <mergeCell ref="W2:Z2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
category check in trophy controller
</commit_message>
<xml_diff>
--- a/doku/Zeitplan.xlsx
+++ b/doku/Zeitplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\IPA-Test-2\doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC53CB5-BB53-4846-99CF-AD275F3B6607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D29F2B3-B0DE-4C7B-BBCC-A289EEAFED72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -300,16 +300,31 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -319,21 +334,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -621,7 +621,7 @@
   <dimension ref="A1:BD46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH44" sqref="AH44"/>
+      <selection activeCell="AL45" sqref="AL45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,166 +632,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16" t="s">
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16" t="s">
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16" t="s">
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16" t="s">
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16" t="s">
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16" t="s">
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16"/>
-      <c r="AI1" s="16" t="s">
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="16"/>
-      <c r="AL1" s="16"/>
-      <c r="AM1" s="16" t="s">
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="AN1" s="16"/>
-      <c r="AO1" s="16"/>
-      <c r="AP1" s="16"/>
-      <c r="AQ1" s="10" t="s">
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="9"/>
+      <c r="AP1" s="9"/>
+      <c r="AQ1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="10"/>
-      <c r="AT1" s="10"/>
-      <c r="AU1" s="10" t="s">
+      <c r="AR1" s="17"/>
+      <c r="AS1" s="17"/>
+      <c r="AT1" s="17"/>
+      <c r="AU1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="AV1" s="10"/>
-      <c r="AW1" s="10"/>
-      <c r="AX1" s="10"/>
+      <c r="AV1" s="17"/>
+      <c r="AW1" s="17"/>
+      <c r="AX1" s="17"/>
     </row>
     <row r="2" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="11">
+      <c r="A2" s="14"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="10">
         <v>44803</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="11">
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="10">
         <v>44804</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="11">
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="10">
         <v>44809</v>
       </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="11">
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="10">
         <v>44810</v>
       </c>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="11">
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="10">
         <v>44811</v>
       </c>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="11">
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="10">
         <v>44817</v>
       </c>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="11">
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="10">
         <v>44818</v>
       </c>
-      <c r="AB2" s="12"/>
-      <c r="AC2" s="12"/>
-      <c r="AD2" s="12"/>
-      <c r="AE2" s="11">
+      <c r="AB2" s="11"/>
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="11"/>
+      <c r="AE2" s="10">
         <v>44823</v>
       </c>
-      <c r="AF2" s="12"/>
-      <c r="AG2" s="12"/>
-      <c r="AH2" s="12"/>
-      <c r="AI2" s="11">
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="11"/>
+      <c r="AH2" s="11"/>
+      <c r="AI2" s="10">
         <v>44824</v>
       </c>
-      <c r="AJ2" s="12"/>
-      <c r="AK2" s="12"/>
-      <c r="AL2" s="12"/>
-      <c r="AM2" s="11">
+      <c r="AJ2" s="11"/>
+      <c r="AK2" s="11"/>
+      <c r="AL2" s="11"/>
+      <c r="AM2" s="10">
         <v>44825</v>
       </c>
-      <c r="AN2" s="12"/>
-      <c r="AO2" s="12"/>
-      <c r="AP2" s="12"/>
-      <c r="AQ2" s="11">
+      <c r="AN2" s="11"/>
+      <c r="AO2" s="11"/>
+      <c r="AP2" s="11"/>
+      <c r="AQ2" s="10">
         <v>44830</v>
       </c>
-      <c r="AR2" s="12"/>
-      <c r="AS2" s="12"/>
-      <c r="AT2" s="12"/>
-      <c r="AU2" s="11">
+      <c r="AR2" s="11"/>
+      <c r="AS2" s="11"/>
+      <c r="AT2" s="11"/>
+      <c r="AU2" s="10">
         <v>44831</v>
       </c>
-      <c r="AV2" s="12"/>
-      <c r="AW2" s="12"/>
-      <c r="AX2" s="12"/>
+      <c r="AV2" s="11"/>
+      <c r="AW2" s="11"/>
+      <c r="AX2" s="11"/>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="5"/>
@@ -844,8 +844,8 @@
       <c r="BD3" s="3"/>
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="9"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="2"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
@@ -861,8 +861,8 @@
       <c r="BD4" s="2"/>
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="4"/>
@@ -877,8 +877,8 @@
       <c r="AX5" s="8"/>
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="9"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="K6" s="8"/>
@@ -891,8 +891,8 @@
       <c r="AX6" s="8"/>
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="12" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="4"/>
@@ -908,8 +908,8 @@
       <c r="AX7" s="8"/>
     </row>
     <row r="8" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="12"/>
       <c r="D8" s="2"/>
       <c r="I8" s="2"/>
       <c r="K8" s="8"/>
@@ -922,10 +922,10 @@
       <c r="AX8" s="8"/>
     </row>
     <row r="9" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="12" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="6"/>
@@ -941,8 +941,8 @@
       <c r="AX9" s="8"/>
     </row>
     <row r="10" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="9"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="12"/>
       <c r="E10" s="2"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
@@ -954,8 +954,8 @@
       <c r="AX10" s="8"/>
     </row>
     <row r="11" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="12" t="s">
         <v>24</v>
       </c>
       <c r="H11" s="6"/>
@@ -970,8 +970,8 @@
       <c r="AX11" s="8"/>
     </row>
     <row r="12" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="9"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="12"/>
       <c r="E12" s="2"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
@@ -983,8 +983,8 @@
       <c r="AX12" s="8"/>
     </row>
     <row r="13" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="16"/>
+      <c r="B13" s="12" t="s">
         <v>26</v>
       </c>
       <c r="I13" s="6"/>
@@ -1000,8 +1000,8 @@
       <c r="AX13" s="8"/>
     </row>
     <row r="14" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="9"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="12"/>
       <c r="F14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1015,8 +1015,8 @@
       <c r="AX14" s="8"/>
     </row>
     <row r="15" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="9" t="s">
+      <c r="A15" s="16"/>
+      <c r="B15" s="12" t="s">
         <v>25</v>
       </c>
       <c r="J15" s="6"/>
@@ -1031,8 +1031,8 @@
       <c r="AX15" s="8"/>
     </row>
     <row r="16" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="9"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="12"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1046,10 +1046,10 @@
       <c r="AX16" s="8"/>
     </row>
     <row r="17" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="12" t="s">
         <v>27</v>
       </c>
       <c r="K17" s="8"/>
@@ -1064,8 +1064,8 @@
       <c r="AX17" s="8"/>
     </row>
     <row r="18" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="9"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="12"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
       <c r="N18" s="2"/>
@@ -1077,8 +1077,8 @@
       <c r="AX18" s="8"/>
     </row>
     <row r="19" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="9" t="s">
+      <c r="A19" s="16"/>
+      <c r="B19" s="12" t="s">
         <v>28</v>
       </c>
       <c r="K19" s="8"/>
@@ -1094,8 +1094,8 @@
       <c r="AX19" s="8"/>
     </row>
     <row r="20" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="9"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="12"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="N20" s="2"/>
@@ -1107,10 +1107,10 @@
       <c r="AX20" s="8"/>
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="12" t="s">
         <v>31</v>
       </c>
       <c r="K21" s="8"/>
@@ -1124,8 +1124,8 @@
       <c r="AX21" s="8"/>
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="9"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="12"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="N22" s="2"/>
@@ -1137,8 +1137,8 @@
       <c r="AX22" s="8"/>
     </row>
     <row r="23" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="9" t="s">
+      <c r="A23" s="16"/>
+      <c r="B23" s="12" t="s">
         <v>32</v>
       </c>
       <c r="K23" s="8"/>
@@ -1153,8 +1153,8 @@
       <c r="AX23" s="8"/>
     </row>
     <row r="24" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="9"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="12"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
       <c r="O24" s="2"/>
@@ -1167,8 +1167,8 @@
       <c r="AX24" s="8"/>
     </row>
     <row r="25" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="9" t="s">
+      <c r="A25" s="16"/>
+      <c r="B25" s="12" t="s">
         <v>33</v>
       </c>
       <c r="K25" s="8"/>
@@ -1183,8 +1183,8 @@
       <c r="AX25" s="8"/>
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="9"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="12"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
       <c r="P26" s="2"/>
@@ -1197,8 +1197,8 @@
       <c r="AX26" s="8"/>
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="9" t="s">
+      <c r="A27" s="16"/>
+      <c r="B27" s="12" t="s">
         <v>34</v>
       </c>
       <c r="K27" s="8"/>
@@ -1212,8 +1212,8 @@
       <c r="AX27" s="8"/>
     </row>
     <row r="28" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="9"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="12"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
       <c r="Q28" s="2"/>
@@ -1226,8 +1226,8 @@
       <c r="AX28" s="8"/>
     </row>
     <row r="29" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="9" t="s">
+      <c r="A29" s="16"/>
+      <c r="B29" s="12" t="s">
         <v>35</v>
       </c>
       <c r="K29" s="8"/>
@@ -1242,8 +1242,8 @@
       <c r="AX29" s="8"/>
     </row>
     <row r="30" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="9"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="12"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
       <c r="S30" s="2"/>
@@ -1256,8 +1256,8 @@
       <c r="AX30" s="8"/>
     </row>
     <row r="31" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="9" t="s">
+      <c r="A31" s="16"/>
+      <c r="B31" s="12" t="s">
         <v>36</v>
       </c>
       <c r="K31" s="8"/>
@@ -1273,8 +1273,8 @@
       <c r="AX31" s="8"/>
     </row>
     <row r="32" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="9"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="12"/>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
       <c r="R32" s="2"/>
@@ -1289,8 +1289,8 @@
       <c r="AX32" s="8"/>
     </row>
     <row r="33" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="B33" s="9" t="s">
+      <c r="A33" s="16"/>
+      <c r="B33" s="12" t="s">
         <v>37</v>
       </c>
       <c r="K33" s="8"/>
@@ -1307,8 +1307,8 @@
       <c r="AX33" s="8"/>
     </row>
     <row r="34" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
-      <c r="B34" s="9"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="12"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
       <c r="W34" s="2"/>
@@ -1322,8 +1322,8 @@
       <c r="AX34" s="8"/>
     </row>
     <row r="35" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
-      <c r="B35" s="9" t="s">
+      <c r="A35" s="16"/>
+      <c r="B35" s="12" t="s">
         <v>38</v>
       </c>
       <c r="K35" s="8"/>
@@ -1341,8 +1341,8 @@
       <c r="AX35" s="8"/>
     </row>
     <row r="36" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="B36" s="9"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="12"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
       <c r="Y36" s="2"/>
@@ -1355,8 +1355,8 @@
       <c r="AX36" s="8"/>
     </row>
     <row r="37" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
-      <c r="B37" s="9" t="s">
+      <c r="A37" s="16"/>
+      <c r="B37" s="12" t="s">
         <v>39</v>
       </c>
       <c r="K37" s="8"/>
@@ -1371,8 +1371,8 @@
       <c r="AX37" s="8"/>
     </row>
     <row r="38" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="12"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
       <c r="AD38" s="2"/>
@@ -1384,10 +1384,10 @@
       <c r="AX38" s="8"/>
     </row>
     <row r="39" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="12" t="s">
         <v>40</v>
       </c>
       <c r="K39" s="8"/>
@@ -1402,8 +1402,8 @@
       <c r="AX39" s="8"/>
     </row>
     <row r="40" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="12"/>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
       <c r="AE40" s="8"/>
@@ -1416,8 +1416,8 @@
       <c r="AX40" s="8"/>
     </row>
     <row r="41" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
-      <c r="B41" s="9" t="s">
+      <c r="A41" s="16"/>
+      <c r="B41" s="12" t="s">
         <v>41</v>
       </c>
       <c r="K41" s="8"/>
@@ -1431,21 +1431,24 @@
       <c r="AX41" s="8"/>
     </row>
     <row r="42" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="12"/>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
       <c r="AE42" s="8"/>
       <c r="AF42" s="8"/>
       <c r="AH42" s="2"/>
+      <c r="AI42" s="2"/>
+      <c r="AJ42" s="2"/>
+      <c r="AK42" s="2"/>
       <c r="AQ42" s="8"/>
       <c r="AR42" s="8"/>
       <c r="AW42" s="8"/>
       <c r="AX42" s="8"/>
     </row>
     <row r="43" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
-      <c r="B43" s="9" t="s">
+      <c r="A43" s="16"/>
+      <c r="B43" s="12" t="s">
         <v>42</v>
       </c>
       <c r="K43" s="8"/>
@@ -1460,23 +1463,27 @@
       <c r="AX43" s="8"/>
     </row>
     <row r="44" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
-      <c r="B44" s="9"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="12"/>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
       <c r="AE44" s="8"/>
       <c r="AF44" s="8"/>
-      <c r="AH44" s="2"/>
+      <c r="AH44" s="6"/>
+      <c r="AI44" s="2"/>
+      <c r="AJ44" s="2"/>
+      <c r="AK44" s="2"/>
+      <c r="AL44" s="2"/>
       <c r="AQ44" s="8"/>
       <c r="AR44" s="8"/>
       <c r="AW44" s="8"/>
       <c r="AX44" s="8"/>
     </row>
     <row r="45" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="12" t="s">
         <v>43</v>
       </c>
       <c r="K45" s="8"/>
@@ -1493,8 +1500,8 @@
       <c r="AX45" s="8"/>
     </row>
     <row r="46" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
-      <c r="B46" s="9"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="12"/>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
       <c r="AE46" s="8"/>
@@ -1506,38 +1513,12 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="AE1:AH1"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="W1:Z1"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="AA1:AD1"/>
-    <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A9:A16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A21:A38"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
     <mergeCell ref="AQ1:AT1"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="AU1:AX1"/>
@@ -1554,12 +1535,38 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="AM1:AP1"/>
     <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:A16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A21:A38"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="AA1:AD1"/>
+    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="AE1:AH1"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="W1:Z1"/>
+    <mergeCell ref="W2:Z2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add power point presentation
</commit_message>
<xml_diff>
--- a/doku/Zeitplan.xlsx
+++ b/doku/Zeitplan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\IPA-Test-2\doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5B6870-2DF1-44B8-A2A0-A8DC5CA13E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C582671-8270-44A4-8139-CEE747DE79B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-5530" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -650,8 +650,8 @@
   </sheetPr>
   <dimension ref="A1:BD46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BC17" sqref="BC17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BF35" sqref="BE35:BF35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1651,6 +1651,8 @@
       <c r="AV46" s="2"/>
       <c r="AW46" s="8"/>
       <c r="AX46" s="8"/>
+      <c r="AY46" s="2"/>
+      <c r="AZ46" s="2"/>
       <c r="BA46" s="8"/>
       <c r="BB46" s="8"/>
     </row>

</xml_diff>